<commit_message>
script to generate covid scenarios
</commit_message>
<xml_diff>
--- a/Somalia-COVID-impact/Inputs_COVID_Malaria_National.xlsx
+++ b/Somalia-COVID-impact/Inputs_COVID_Malaria_National.xlsx
@@ -1,39 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060A8C8F-FA22-8B4E-B121-CA23B0BE5578}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="National" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
+    <t>Parameter</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
+    <t>nu</t>
+  </si>
+  <si>
     <t>alpha</t>
   </si>
   <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>nu</t>
-  </si>
-  <si>
     <t>lambda</t>
   </si>
   <si>
@@ -46,6 +40,9 @@
     <t>zeta</t>
   </si>
   <si>
+    <t>r</t>
+  </si>
+  <si>
     <t>b</t>
   </si>
   <si>
@@ -88,7 +85,7 @@
     <t>disease-induced death rate</t>
   </si>
   <si>
-    <t>r</t>
+    <t>depends on the transmission probabilities, the man biting rate of the mosquitoes, the carrying capacities of the environment for both species as well as on the ratio between the vector and human populations</t>
   </si>
   <si>
     <t>This gives the transmission rate from human to vector to be about 0.4167</t>
@@ -116,19 +113,13 @@
   </si>
   <si>
     <t>infected mosquitoes</t>
-  </si>
-  <si>
-    <t>depends on the transmission probabilities, the man biting rate of the mosquitoes, the carrying capacities of the environment for both species as well as on the ratio between the vector and human populations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,13 +135,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -160,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -168,30 +152,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -206,44 +196,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -270,15 +260,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -305,7 +294,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -317,342 +305,359 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.83203125" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1.07056751</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>1.0705675100000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>0.79798172999999994</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+        <v>0.7979817299999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>1.8400000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+        <v>0.00184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>0.35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6">
-        <v>1.1000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+        <v>0.0012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>4.8792</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>5.692399999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>2.4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12">
-        <v>1.1022000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>1.2024</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>0.98</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.26610852000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>0.26610852</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15">
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16">
-        <v>11.733688900000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>11.7336889</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>5.79356443</v>
@@ -660,6 +665,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>